<commit_message>
Changed LED resistor value
</commit_message>
<xml_diff>
--- a/schematic/BOM.xlsx
+++ b/schematic/BOM.xlsx
@@ -91,9 +91,6 @@
     <t>LED_blue</t>
   </si>
   <si>
-    <t>RESISTOR, 130Ω</t>
-  </si>
-  <si>
     <t>RESISTOR, 30Ω</t>
   </si>
   <si>
@@ -290,6 +287,9 @@
   </si>
   <si>
     <t>Xtal, Osc 24 MHz</t>
+  </si>
+  <si>
+    <t>RESISTOR, 120Ω</t>
   </si>
 </sst>
 </file>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -653,19 +653,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" t="s">
         <v>87</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>88</v>
-      </c>
-      <c r="E1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -676,10 +676,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="86.4">
@@ -690,10 +690,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -704,10 +704,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -718,10 +718,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2">
@@ -732,10 +732,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -746,10 +746,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -760,10 +760,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -771,13 +771,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -788,10 +788,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -802,10 +802,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -816,10 +816,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -830,10 +830,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -844,10 +844,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -858,10 +858,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -872,10 +872,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -886,10 +886,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -900,10 +900,10 @@
         <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="43.2">
@@ -914,10 +914,10 @@
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -928,10 +928,10 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -942,10 +942,10 @@
         <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -956,10 +956,10 @@
         <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -970,10 +970,10 @@
         <v>20</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -984,10 +984,10 @@
         <v>21</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -998,10 +998,10 @@
         <v>22</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1012,10 +1012,10 @@
         <v>23</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1026,10 +1026,10 @@
         <v>24</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1037,13 +1037,13 @@
         <v>1</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1051,13 +1051,13 @@
         <v>3</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1065,13 +1065,13 @@
         <v>2</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1079,13 +1079,13 @@
         <v>2</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1093,13 +1093,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1107,13 +1107,13 @@
         <v>1</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1121,13 +1121,13 @@
         <v>1</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>